<commit_message>
add order quantities to bom
</commit_message>
<xml_diff>
--- a/pcb/polytag/rev_a/polytag_bom.xlsx
+++ b/pcb/polytag/rev_a/polytag_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="118" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="113" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="130">
   <si>
     <t>Qty</t>
   </si>
@@ -47,6 +47,15 @@
     <t>RICHARDSON_RFPD</t>
   </si>
   <si>
+    <t>Needed</t>
+  </si>
+  <si>
+    <t>Order 2015-07-30</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
     <t>TAIYO-YUDEN-AH086M</t>
   </si>
   <si>
@@ -149,7 +158,7 @@
     <t>C7, C8, C9, C10</t>
   </si>
   <si>
-    <t>490-1318-6-ND</t>
+    <t>490-1318-1-ND</t>
   </si>
   <si>
     <t>0.47uF</t>
@@ -194,6 +203,9 @@
     <t>LEDs</t>
   </si>
   <si>
+    <t>160-1446-1-ND</t>
+  </si>
+  <si>
     <t>BLUE</t>
   </si>
   <si>
@@ -390,6 +402,9 @@
   </si>
   <si>
     <t>887-2003-1-ND</t>
+  </si>
+  <si>
+    <t>Wanted</t>
   </si>
 </sst>
 </file>
@@ -399,11 +414,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -421,10 +437,18 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -451,7 +475,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -475,13 +499,16 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -490,14 +517,26 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Untitled1" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -506,10 +545,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -518,12 +557,12 @@
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="36.4489795918367"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.6122448979592"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="75.0714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.984693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="30.984693877551"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.7142857142857"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.65816326530612"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="15.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -557,28 +596,48 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <f aca="false">A2*$I$32</f>
+        <v>108</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <f aca="false">L2-K2</f>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,22 +645,30 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">A3*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <f aca="false">L3-K3</f>
+        <v>-36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,25 +676,33 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">A4*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <f aca="false">L4-K4</f>
+        <v>-36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,22 +710,33 @@
         <v>1</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">A5*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <f aca="false">L5-K5</f>
+        <v>864</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,22 +744,30 @@
         <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>28</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">A6*$I$32</f>
+        <v>72</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">L6-K6</f>
+        <v>-72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -681,22 +775,30 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">A7*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">L7-K7</f>
+        <v>-36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -704,22 +806,33 @@
         <v>1</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">A8*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <f aca="false">L8-K8</f>
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,22 +840,33 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">A9*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <f aca="false">L9-K9</f>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -750,22 +874,33 @@
         <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">A10*$I$32</f>
+        <v>144</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false">L10-K10</f>
+        <v>356</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,22 +908,33 @@
         <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">A11*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <f aca="false">L11-K11</f>
+        <v>464</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,22 +942,33 @@
         <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <f aca="false">A12*$I$32</f>
+        <v>72</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <f aca="false">L12-K12</f>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,22 +976,33 @@
         <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <f aca="false">A13*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <f aca="false">L13-K13</f>
+        <v>47</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,19 +1010,33 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">A14*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <f aca="false">L14-K14</f>
+        <v>464</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,22 +1044,33 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="E15" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">A15*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <f aca="false">L15-K15</f>
+        <v>4</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -885,28 +1078,39 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E16" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <f aca="false">A16*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <f aca="false">L16-K16</f>
         <v>64</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,22 +1118,33 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <f aca="false">A17*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <f aca="false">L17-K17</f>
+        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,22 +1152,33 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <f aca="false">A18*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L18" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>79</v>
+      <c r="M18" s="0" t="n">
+        <f aca="false">L18-K18</f>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -960,22 +1186,33 @@
         <v>2</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <f aca="false">A19*$I$32</f>
+        <v>72</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <f aca="false">L19-K19</f>
         <v>81</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,22 +1220,33 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>82</v>
-      </c>
       <c r="E20" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <f aca="false">A20*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <f aca="false">L20-K20</f>
+        <v>464</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,22 +1254,33 @@
         <v>2</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <f aca="false">A21*$I$32</f>
+        <v>72</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <f aca="false">L21-K21</f>
+        <v>678</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,22 +1288,33 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <f aca="false">A22*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <f aca="false">L22-K22</f>
+        <v>44</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,22 +1322,33 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <f aca="false">A23*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <f aca="false">L23-K23</f>
+        <v>464</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,22 +1356,33 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <f aca="false">A24*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <f aca="false">L24-K24</f>
+        <v>464</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,25 +1390,33 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <f aca="false">A25*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <f aca="false">L25-K25</f>
+        <v>-36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1124,19 +1424,30 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <f aca="false">A26*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <f aca="false">L26-K26</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,22 +1455,33 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <f aca="false">A27*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <f aca="false">L27-K27</f>
+        <v>64</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,22 +1489,33 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <f aca="false">A28*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <f aca="false">L28-K28</f>
+        <v>64</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,25 +1523,49 @@
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <f aca="false">A29*$I$32</f>
+        <v>36</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <f aca="false">L29-K29</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H32" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="M2:M29">
+    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>